<commit_message>
Antes de mudar a interface gráfica novamente.
</commit_message>
<xml_diff>
--- a/dados_mensais/Produtividade - 02.2025.xlsx
+++ b/dados_mensais/Produtividade - 02.2025.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b1b28a1440785203/Área de Trabalho/Programa Analyzer/Projeto Analisador de Produção/Projeto-APROD/dados_mensais/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_280D43EBD723092C812C4CEDC5E800B7797A623B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0459B32C-C90E-42F5-B399-459E79460DA0}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-19310" yWindow="520" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -2458,8 +2464,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2522,13 +2528,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2566,7 +2580,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -2600,6 +2614,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -2634,9 +2649,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2809,14 +2825,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H392"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="92.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2842,7 +2862,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -2868,7 +2888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2894,7 +2914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -2920,7 +2940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2946,7 +2966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -2972,7 +2992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -2998,7 +3018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -3024,7 +3044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -3050,7 +3070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -3076,7 +3096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -3102,7 +3122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -3128,7 +3148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -3154,7 +3174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -3180,7 +3200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -3206,7 +3226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -3232,7 +3252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -3258,7 +3278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -3284,7 +3304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -3310,7 +3330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -3336,7 +3356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -3362,7 +3382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -3388,7 +3408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -3414,7 +3434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -3440,7 +3460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -3466,7 +3486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -3492,7 +3512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -3518,7 +3538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -3544,7 +3564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -3570,7 +3590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -3596,7 +3616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -3622,7 +3642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>8</v>
       </c>
@@ -3648,7 +3668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>8</v>
       </c>
@@ -3674,7 +3694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>8</v>
       </c>
@@ -3700,7 +3720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>8</v>
       </c>
@@ -3726,7 +3746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>8</v>
       </c>
@@ -3752,7 +3772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>8</v>
       </c>
@@ -3778,7 +3798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>8</v>
       </c>
@@ -3804,7 +3824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>8</v>
       </c>
@@ -3830,7 +3850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>8</v>
       </c>
@@ -3856,7 +3876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>8</v>
       </c>
@@ -3882,7 +3902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>8</v>
       </c>
@@ -3908,7 +3928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>8</v>
       </c>
@@ -3934,7 +3954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>8</v>
       </c>
@@ -3960,7 +3980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>8</v>
       </c>
@@ -3986,7 +4006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>8</v>
       </c>
@@ -4012,7 +4032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>8</v>
       </c>
@@ -4038,7 +4058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>8</v>
       </c>
@@ -4064,7 +4084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>8</v>
       </c>
@@ -4090,7 +4110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>8</v>
       </c>
@@ -4116,7 +4136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>8</v>
       </c>
@@ -4142,7 +4162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>8</v>
       </c>
@@ -4168,7 +4188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>8</v>
       </c>
@@ -4194,7 +4214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>8</v>
       </c>
@@ -4220,7 +4240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>8</v>
       </c>
@@ -4246,7 +4266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>8</v>
       </c>
@@ -4272,7 +4292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>8</v>
       </c>
@@ -4298,7 +4318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>8</v>
       </c>
@@ -4324,7 +4344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>8</v>
       </c>
@@ -4350,7 +4370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>8</v>
       </c>
@@ -4376,7 +4396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>8</v>
       </c>
@@ -4402,7 +4422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>8</v>
       </c>
@@ -4428,7 +4448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>8</v>
       </c>
@@ -4454,7 +4474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>8</v>
       </c>
@@ -4480,7 +4500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>8</v>
       </c>
@@ -4506,7 +4526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>8</v>
       </c>
@@ -4532,7 +4552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>8</v>
       </c>
@@ -4558,7 +4578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>8</v>
       </c>
@@ -4584,7 +4604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>8</v>
       </c>
@@ -4610,7 +4630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>8</v>
       </c>
@@ -4636,7 +4656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>8</v>
       </c>
@@ -4662,7 +4682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>8</v>
       </c>
@@ -4688,7 +4708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>8</v>
       </c>
@@ -4714,7 +4734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>8</v>
       </c>
@@ -4740,7 +4760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>8</v>
       </c>
@@ -4766,7 +4786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>8</v>
       </c>
@@ -4792,7 +4812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>8</v>
       </c>
@@ -4818,7 +4838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>8</v>
       </c>
@@ -4844,7 +4864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>8</v>
       </c>
@@ -4870,7 +4890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>8</v>
       </c>
@@ -4896,7 +4916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>8</v>
       </c>
@@ -4922,7 +4942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>8</v>
       </c>
@@ -4948,7 +4968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>8</v>
       </c>
@@ -4974,7 +4994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>8</v>
       </c>
@@ -5000,7 +5020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>8</v>
       </c>
@@ -5026,7 +5046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>8</v>
       </c>
@@ -5052,7 +5072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>8</v>
       </c>
@@ -5078,7 +5098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>8</v>
       </c>
@@ -5104,7 +5124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>8</v>
       </c>
@@ -5130,7 +5150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>8</v>
       </c>
@@ -5156,7 +5176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>8</v>
       </c>
@@ -5182,7 +5202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>8</v>
       </c>
@@ -5208,7 +5228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>8</v>
       </c>
@@ -5234,7 +5254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>8</v>
       </c>
@@ -5260,7 +5280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>8</v>
       </c>
@@ -5286,7 +5306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>8</v>
       </c>
@@ -5312,7 +5332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>8</v>
       </c>
@@ -5338,7 +5358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>8</v>
       </c>
@@ -5364,7 +5384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>8</v>
       </c>
@@ -5390,7 +5410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>8</v>
       </c>
@@ -5416,7 +5436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:8">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>8</v>
       </c>
@@ -5442,7 +5462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:8">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>8</v>
       </c>
@@ -5468,7 +5488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:8">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>8</v>
       </c>
@@ -5494,7 +5514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:8">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>8</v>
       </c>
@@ -5520,7 +5540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:8">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>8</v>
       </c>
@@ -5546,7 +5566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:8">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>8</v>
       </c>
@@ -5572,7 +5592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:8">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>8</v>
       </c>
@@ -5598,7 +5618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:8">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>8</v>
       </c>
@@ -5624,7 +5644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:8">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>8</v>
       </c>
@@ -5650,7 +5670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:8">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>8</v>
       </c>
@@ -5676,7 +5696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:8">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>8</v>
       </c>
@@ -5702,7 +5722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:8">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>8</v>
       </c>
@@ -5728,7 +5748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:8">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>8</v>
       </c>
@@ -5754,7 +5774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:8">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>8</v>
       </c>
@@ -5780,7 +5800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:8">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>8</v>
       </c>
@@ -5806,7 +5826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:8">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>8</v>
       </c>
@@ -5832,7 +5852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:8">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>8</v>
       </c>
@@ -5858,7 +5878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:8">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>8</v>
       </c>
@@ -5884,7 +5904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:8">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>8</v>
       </c>
@@ -5910,7 +5930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:8">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>8</v>
       </c>
@@ -5936,7 +5956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:8">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>8</v>
       </c>
@@ -5962,7 +5982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:8">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>8</v>
       </c>
@@ -5988,7 +6008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:8">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>8</v>
       </c>
@@ -6014,7 +6034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:8">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>8</v>
       </c>
@@ -6040,7 +6060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:8">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>8</v>
       </c>
@@ -6066,7 +6086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:8">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>8</v>
       </c>
@@ -6092,7 +6112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:8">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>8</v>
       </c>
@@ -6118,7 +6138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:8">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>8</v>
       </c>
@@ -6144,7 +6164,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:8">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>8</v>
       </c>
@@ -6170,7 +6190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:8">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>8</v>
       </c>
@@ -6196,7 +6216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:8">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>8</v>
       </c>
@@ -6222,7 +6242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:8">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>8</v>
       </c>
@@ -6248,7 +6268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:8">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>8</v>
       </c>
@@ -6274,7 +6294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:8">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>8</v>
       </c>
@@ -6300,7 +6320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:8">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>8</v>
       </c>
@@ -6326,7 +6346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:8">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>8</v>
       </c>
@@ -6352,7 +6372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:8">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>8</v>
       </c>
@@ -6378,7 +6398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:8">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>8</v>
       </c>
@@ -6404,7 +6424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:8">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>8</v>
       </c>
@@ -6430,7 +6450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:8">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>8</v>
       </c>
@@ -6456,7 +6476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:8">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>8</v>
       </c>
@@ -6482,7 +6502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:8">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>8</v>
       </c>
@@ -6508,7 +6528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:8">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>8</v>
       </c>
@@ -6534,7 +6554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:8">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>8</v>
       </c>
@@ -6560,7 +6580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:8">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>8</v>
       </c>
@@ -6586,7 +6606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:8">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>8</v>
       </c>
@@ -6612,7 +6632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:8">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>8</v>
       </c>
@@ -6638,7 +6658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:8">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>8</v>
       </c>
@@ -6664,7 +6684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:8">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>8</v>
       </c>
@@ -6690,7 +6710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:8">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>8</v>
       </c>
@@ -6716,7 +6736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:8">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>8</v>
       </c>
@@ -6742,7 +6762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:8">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>8</v>
       </c>
@@ -6768,7 +6788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:8">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>8</v>
       </c>
@@ -6794,7 +6814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:8">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>8</v>
       </c>
@@ -6820,7 +6840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:8">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>8</v>
       </c>
@@ -6846,7 +6866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:8">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>8</v>
       </c>
@@ -6872,7 +6892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:8">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>8</v>
       </c>
@@ -6898,7 +6918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:8">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>8</v>
       </c>
@@ -6924,7 +6944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:8">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>8</v>
       </c>
@@ -6950,7 +6970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:8">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>8</v>
       </c>
@@ -6976,7 +6996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:8">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>8</v>
       </c>
@@ -7002,7 +7022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:8">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>8</v>
       </c>
@@ -7028,7 +7048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:8">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>8</v>
       </c>
@@ -7054,7 +7074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:8">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>8</v>
       </c>
@@ -7080,7 +7100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:8">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>8</v>
       </c>
@@ -7106,7 +7126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:8">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>8</v>
       </c>
@@ -7132,7 +7152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:8">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>8</v>
       </c>
@@ -7158,7 +7178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:8">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>8</v>
       </c>
@@ -7184,7 +7204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:8">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>8</v>
       </c>
@@ -7210,7 +7230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:8">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>8</v>
       </c>
@@ -7236,7 +7256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:8">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>8</v>
       </c>
@@ -7262,7 +7282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:8">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>8</v>
       </c>
@@ -7288,7 +7308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:8">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>8</v>
       </c>
@@ -7314,7 +7334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:8">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>8</v>
       </c>
@@ -7340,7 +7360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:8">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>8</v>
       </c>
@@ -7366,7 +7386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:8">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>8</v>
       </c>
@@ -7392,7 +7412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:8">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>8</v>
       </c>
@@ -7418,7 +7438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:8">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>8</v>
       </c>
@@ -7444,7 +7464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:8">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>8</v>
       </c>
@@ -7470,7 +7490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:8">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>8</v>
       </c>
@@ -7496,7 +7516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:8">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>8</v>
       </c>
@@ -7522,7 +7542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:8">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>8</v>
       </c>
@@ -7548,7 +7568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:8">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>8</v>
       </c>
@@ -7574,7 +7594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:8">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>8</v>
       </c>
@@ -7600,7 +7620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:8">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>8</v>
       </c>
@@ -7626,7 +7646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:8">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>8</v>
       </c>
@@ -7652,7 +7672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:8">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>8</v>
       </c>
@@ -7678,7 +7698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:8">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>8</v>
       </c>
@@ -7704,7 +7724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:8">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>8</v>
       </c>
@@ -7730,7 +7750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:8">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>8</v>
       </c>
@@ -7756,7 +7776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:8">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>8</v>
       </c>
@@ -7782,7 +7802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:8">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>8</v>
       </c>
@@ -7808,7 +7828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:8">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>8</v>
       </c>
@@ -7834,7 +7854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:8">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>8</v>
       </c>
@@ -7860,7 +7880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:8">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>8</v>
       </c>
@@ -7886,7 +7906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:8">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>8</v>
       </c>
@@ -7912,7 +7932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:8">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>8</v>
       </c>
@@ -7938,7 +7958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:8">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>8</v>
       </c>
@@ -7964,7 +7984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:8">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>8</v>
       </c>
@@ -7990,7 +8010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:8">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>8</v>
       </c>
@@ -8016,7 +8036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:8">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>8</v>
       </c>
@@ -8042,7 +8062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:8">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>8</v>
       </c>
@@ -8068,7 +8088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:8">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>8</v>
       </c>
@@ -8094,7 +8114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:8">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>8</v>
       </c>
@@ -8120,7 +8140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:8">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>8</v>
       </c>
@@ -8146,7 +8166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:8">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>8</v>
       </c>
@@ -8172,7 +8192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:8">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>8</v>
       </c>
@@ -8198,7 +8218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:8">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>8</v>
       </c>
@@ -8224,7 +8244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:8">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>8</v>
       </c>
@@ -8250,7 +8270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:8">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>8</v>
       </c>
@@ -8276,7 +8296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:8">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>8</v>
       </c>
@@ -8302,7 +8322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:8">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>8</v>
       </c>
@@ -8328,7 +8348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:8">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>8</v>
       </c>
@@ -8354,7 +8374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:8">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>8</v>
       </c>
@@ -8380,7 +8400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:8">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>8</v>
       </c>
@@ -8406,7 +8426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:8">
+    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>8</v>
       </c>
@@ -8432,7 +8452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="1:8">
+    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>8</v>
       </c>
@@ -8458,7 +8478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:8">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>8</v>
       </c>
@@ -8484,7 +8504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:8">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>8</v>
       </c>
@@ -8510,7 +8530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="220" spans="1:8">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>8</v>
       </c>
@@ -8536,7 +8556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:8">
+    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>8</v>
       </c>
@@ -8562,7 +8582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:8">
+    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>8</v>
       </c>
@@ -8588,7 +8608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:8">
+    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>8</v>
       </c>
@@ -8614,7 +8634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:8">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>8</v>
       </c>
@@ -8640,7 +8660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="1:8">
+    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>8</v>
       </c>
@@ -8666,7 +8686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="226" spans="1:8">
+    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>8</v>
       </c>
@@ -8692,7 +8712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:8">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>8</v>
       </c>
@@ -8718,7 +8738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:8">
+    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>9</v>
       </c>
@@ -8741,7 +8761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="1:8">
+    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>10</v>
       </c>
@@ -8767,7 +8787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:8">
+    <row r="230" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>10</v>
       </c>
@@ -8793,7 +8813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:8">
+    <row r="231" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>10</v>
       </c>
@@ -8819,7 +8839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:8">
+    <row r="232" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>10</v>
       </c>
@@ -8845,7 +8865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="1:8">
+    <row r="233" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>10</v>
       </c>
@@ -8871,7 +8891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:8">
+    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>10</v>
       </c>
@@ -8897,7 +8917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="235" spans="1:8">
+    <row r="235" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>10</v>
       </c>
@@ -8923,7 +8943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="236" spans="1:8">
+    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>10</v>
       </c>
@@ -8949,7 +8969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="237" spans="1:8">
+    <row r="237" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>10</v>
       </c>
@@ -8975,7 +8995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="238" spans="1:8">
+    <row r="238" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>10</v>
       </c>
@@ -9001,7 +9021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:8">
+    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>10</v>
       </c>
@@ -9027,7 +9047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="240" spans="1:8">
+    <row r="240" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>10</v>
       </c>
@@ -9053,7 +9073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="241" spans="1:8">
+    <row r="241" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>10</v>
       </c>
@@ -9079,7 +9099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="242" spans="1:8">
+    <row r="242" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>10</v>
       </c>
@@ -9102,7 +9122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:8">
+    <row r="243" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>10</v>
       </c>
@@ -9128,7 +9148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="244" spans="1:8">
+    <row r="244" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>10</v>
       </c>
@@ -9154,7 +9174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="245" spans="1:8">
+    <row r="245" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>10</v>
       </c>
@@ -9180,7 +9200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:8">
+    <row r="246" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>10</v>
       </c>
@@ -9206,7 +9226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="247" spans="1:8">
+    <row r="247" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>10</v>
       </c>
@@ -9229,7 +9249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:8">
+    <row r="248" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>10</v>
       </c>
@@ -9255,7 +9275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="249" spans="1:8">
+    <row r="249" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>10</v>
       </c>
@@ -9281,7 +9301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="250" spans="1:8">
+    <row r="250" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>10</v>
       </c>
@@ -9307,7 +9327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="251" spans="1:8">
+    <row r="251" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>10</v>
       </c>
@@ -9333,7 +9353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="252" spans="1:8">
+    <row r="252" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>10</v>
       </c>
@@ -9359,7 +9379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="253" spans="1:8">
+    <row r="253" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>10</v>
       </c>
@@ -9385,7 +9405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="254" spans="1:8">
+    <row r="254" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>10</v>
       </c>
@@ -9411,7 +9431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="255" spans="1:8">
+    <row r="255" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>10</v>
       </c>
@@ -9437,7 +9457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="256" spans="1:8">
+    <row r="256" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>10</v>
       </c>
@@ -9463,7 +9483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="257" spans="1:8">
+    <row r="257" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>10</v>
       </c>
@@ -9489,7 +9509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="258" spans="1:8">
+    <row r="258" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>10</v>
       </c>
@@ -9515,7 +9535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="259" spans="1:8">
+    <row r="259" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>10</v>
       </c>
@@ -9541,7 +9561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="260" spans="1:8">
+    <row r="260" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>10</v>
       </c>
@@ -9567,7 +9587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="261" spans="1:8">
+    <row r="261" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>10</v>
       </c>
@@ -9593,7 +9613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="262" spans="1:8">
+    <row r="262" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>10</v>
       </c>
@@ -9619,7 +9639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="263" spans="1:8">
+    <row r="263" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>10</v>
       </c>
@@ -9645,7 +9665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="264" spans="1:8">
+    <row r="264" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>10</v>
       </c>
@@ -9671,7 +9691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="265" spans="1:8">
+    <row r="265" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>10</v>
       </c>
@@ -9697,7 +9717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="266" spans="1:8">
+    <row r="266" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>10</v>
       </c>
@@ -9723,7 +9743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="267" spans="1:8">
+    <row r="267" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>10</v>
       </c>
@@ -9749,7 +9769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="268" spans="1:8">
+    <row r="268" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>10</v>
       </c>
@@ -9775,7 +9795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="269" spans="1:8">
+    <row r="269" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>10</v>
       </c>
@@ -9801,7 +9821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="270" spans="1:8">
+    <row r="270" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>10</v>
       </c>
@@ -9827,7 +9847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="271" spans="1:8">
+    <row r="271" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>10</v>
       </c>
@@ -9853,7 +9873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="1:8">
+    <row r="272" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>10</v>
       </c>
@@ -9879,7 +9899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="273" spans="1:8">
+    <row r="273" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>10</v>
       </c>
@@ -9905,7 +9925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="274" spans="1:8">
+    <row r="274" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>10</v>
       </c>
@@ -9931,7 +9951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="1:8">
+    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>10</v>
       </c>
@@ -9957,7 +9977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="276" spans="1:8">
+    <row r="276" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>10</v>
       </c>
@@ -9983,7 +10003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="277" spans="1:8">
+    <row r="277" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>10</v>
       </c>
@@ -10009,7 +10029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="278" spans="1:8">
+    <row r="278" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>10</v>
       </c>
@@ -10035,7 +10055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:8">
+    <row r="279" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>10</v>
       </c>
@@ -10061,7 +10081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="280" spans="1:8">
+    <row r="280" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>10</v>
       </c>
@@ -10087,7 +10107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="281" spans="1:8">
+    <row r="281" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>10</v>
       </c>
@@ -10113,7 +10133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="282" spans="1:8">
+    <row r="282" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>10</v>
       </c>
@@ -10139,7 +10159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="283" spans="1:8">
+    <row r="283" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>10</v>
       </c>
@@ -10165,7 +10185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="284" spans="1:8">
+    <row r="284" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>10</v>
       </c>
@@ -10191,7 +10211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="285" spans="1:8">
+    <row r="285" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>10</v>
       </c>
@@ -10217,7 +10237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="286" spans="1:8">
+    <row r="286" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>10</v>
       </c>
@@ -10243,7 +10263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="287" spans="1:8">
+    <row r="287" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>10</v>
       </c>
@@ -10269,7 +10289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="288" spans="1:8">
+    <row r="288" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>10</v>
       </c>
@@ -10295,7 +10315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="289" spans="1:8">
+    <row r="289" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>10</v>
       </c>
@@ -10321,7 +10341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="290" spans="1:8">
+    <row r="290" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>10</v>
       </c>
@@ -10347,7 +10367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="291" spans="1:8">
+    <row r="291" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>10</v>
       </c>
@@ -10373,7 +10393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="292" spans="1:8">
+    <row r="292" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>10</v>
       </c>
@@ -10399,7 +10419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="293" spans="1:8">
+    <row r="293" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>10</v>
       </c>
@@ -10425,7 +10445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="294" spans="1:8">
+    <row r="294" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>10</v>
       </c>
@@ -10448,7 +10468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="295" spans="1:8">
+    <row r="295" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>10</v>
       </c>
@@ -10474,7 +10494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="296" spans="1:8">
+    <row r="296" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>10</v>
       </c>
@@ -10500,7 +10520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="297" spans="1:8">
+    <row r="297" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>10</v>
       </c>
@@ -10523,7 +10543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="298" spans="1:8">
+    <row r="298" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>10</v>
       </c>
@@ -10546,7 +10566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="299" spans="1:8">
+    <row r="299" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>10</v>
       </c>
@@ -10572,7 +10592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="300" spans="1:8">
+    <row r="300" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>10</v>
       </c>
@@ -10595,7 +10615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="301" spans="1:8">
+    <row r="301" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>10</v>
       </c>
@@ -10621,7 +10641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="302" spans="1:8">
+    <row r="302" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>10</v>
       </c>
@@ -10647,7 +10667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="303" spans="1:8">
+    <row r="303" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>10</v>
       </c>
@@ -10673,7 +10693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="304" spans="1:8">
+    <row r="304" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>10</v>
       </c>
@@ -10699,7 +10719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="305" spans="1:8">
+    <row r="305" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>10</v>
       </c>
@@ -10722,7 +10742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="306" spans="1:8">
+    <row r="306" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>10</v>
       </c>
@@ -10748,7 +10768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="307" spans="1:8">
+    <row r="307" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>10</v>
       </c>
@@ -10774,7 +10794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="308" spans="1:8">
+    <row r="308" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>10</v>
       </c>
@@ -10797,7 +10817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="309" spans="1:8">
+    <row r="309" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>10</v>
       </c>
@@ -10823,7 +10843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="310" spans="1:8">
+    <row r="310" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>10</v>
       </c>
@@ -10849,7 +10869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="311" spans="1:8">
+    <row r="311" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>10</v>
       </c>
@@ -10875,7 +10895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="312" spans="1:8">
+    <row r="312" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>10</v>
       </c>
@@ -10901,7 +10921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="313" spans="1:8">
+    <row r="313" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>10</v>
       </c>
@@ -10927,7 +10947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="314" spans="1:8">
+    <row r="314" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>10</v>
       </c>
@@ -10953,7 +10973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="315" spans="1:8">
+    <row r="315" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>10</v>
       </c>
@@ -10976,7 +10996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="316" spans="1:8">
+    <row r="316" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>10</v>
       </c>
@@ -11002,7 +11022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="317" spans="1:8">
+    <row r="317" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>10</v>
       </c>
@@ -11028,7 +11048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="318" spans="1:8">
+    <row r="318" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>10</v>
       </c>
@@ -11054,7 +11074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="319" spans="1:8">
+    <row r="319" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>10</v>
       </c>
@@ -11080,7 +11100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="320" spans="1:8">
+    <row r="320" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>10</v>
       </c>
@@ -11106,7 +11126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="321" spans="1:8">
+    <row r="321" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>10</v>
       </c>
@@ -11129,7 +11149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="322" spans="1:8">
+    <row r="322" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>10</v>
       </c>
@@ -11155,7 +11175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="323" spans="1:8">
+    <row r="323" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>10</v>
       </c>
@@ -11181,7 +11201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="324" spans="1:8">
+    <row r="324" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>10</v>
       </c>
@@ -11207,7 +11227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="325" spans="1:8">
+    <row r="325" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>10</v>
       </c>
@@ -11233,7 +11253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="326" spans="1:8">
+    <row r="326" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>10</v>
       </c>
@@ -11259,7 +11279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="327" spans="1:8">
+    <row r="327" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>10</v>
       </c>
@@ -11285,7 +11305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="328" spans="1:8">
+    <row r="328" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>10</v>
       </c>
@@ -11311,7 +11331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="329" spans="1:8">
+    <row r="329" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>10</v>
       </c>
@@ -11334,7 +11354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="330" spans="1:8">
+    <row r="330" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>10</v>
       </c>
@@ -11360,7 +11380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="331" spans="1:8">
+    <row r="331" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>10</v>
       </c>
@@ -11386,7 +11406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="332" spans="1:8">
+    <row r="332" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>10</v>
       </c>
@@ -11412,7 +11432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="333" spans="1:8">
+    <row r="333" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>10</v>
       </c>
@@ -11438,7 +11458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="334" spans="1:8">
+    <row r="334" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>10</v>
       </c>
@@ -11464,7 +11484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="335" spans="1:8">
+    <row r="335" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>10</v>
       </c>
@@ -11490,7 +11510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="336" spans="1:8">
+    <row r="336" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>10</v>
       </c>
@@ -11513,7 +11533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="337" spans="1:8">
+    <row r="337" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>10</v>
       </c>
@@ -11539,7 +11559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="338" spans="1:8">
+    <row r="338" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>10</v>
       </c>
@@ -11565,7 +11585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="339" spans="1:8">
+    <row r="339" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>10</v>
       </c>
@@ -11591,7 +11611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="340" spans="1:8">
+    <row r="340" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>10</v>
       </c>
@@ -11617,7 +11637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="341" spans="1:8">
+    <row r="341" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>10</v>
       </c>
@@ -11643,7 +11663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="342" spans="1:8">
+    <row r="342" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>10</v>
       </c>
@@ -11669,7 +11689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="343" spans="1:8">
+    <row r="343" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>10</v>
       </c>
@@ -11695,7 +11715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="344" spans="1:8">
+    <row r="344" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>10</v>
       </c>
@@ -11721,7 +11741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="345" spans="1:8">
+    <row r="345" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>10</v>
       </c>
@@ -11747,7 +11767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="346" spans="1:8">
+    <row r="346" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>10</v>
       </c>
@@ -11773,7 +11793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="347" spans="1:8">
+    <row r="347" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>10</v>
       </c>
@@ -11796,7 +11816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="348" spans="1:8">
+    <row r="348" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>10</v>
       </c>
@@ -11822,7 +11842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="349" spans="1:8">
+    <row r="349" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>10</v>
       </c>
@@ -11848,7 +11868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="350" spans="1:8">
+    <row r="350" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>10</v>
       </c>
@@ -11874,7 +11894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="351" spans="1:8">
+    <row r="351" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>10</v>
       </c>
@@ -11900,7 +11920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="352" spans="1:8">
+    <row r="352" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>10</v>
       </c>
@@ -11923,7 +11943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="353" spans="1:8">
+    <row r="353" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>10</v>
       </c>
@@ -11949,7 +11969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="354" spans="1:8">
+    <row r="354" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>10</v>
       </c>
@@ -11975,7 +11995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="355" spans="1:8">
+    <row r="355" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>10</v>
       </c>
@@ -12001,7 +12021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="356" spans="1:8">
+    <row r="356" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>10</v>
       </c>
@@ -12027,7 +12047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="357" spans="1:8">
+    <row r="357" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>10</v>
       </c>
@@ -12053,7 +12073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="358" spans="1:8">
+    <row r="358" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>10</v>
       </c>
@@ -12079,7 +12099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="359" spans="1:8">
+    <row r="359" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>10</v>
       </c>
@@ -12105,7 +12125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="360" spans="1:8">
+    <row r="360" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>10</v>
       </c>
@@ -12131,7 +12151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="361" spans="1:8">
+    <row r="361" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>10</v>
       </c>
@@ -12157,7 +12177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="362" spans="1:8">
+    <row r="362" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>10</v>
       </c>
@@ -12183,7 +12203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="363" spans="1:8">
+    <row r="363" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>10</v>
       </c>
@@ -12209,7 +12229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="364" spans="1:8">
+    <row r="364" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>10</v>
       </c>
@@ -12235,7 +12255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="365" spans="1:8">
+    <row r="365" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>10</v>
       </c>
@@ -12261,7 +12281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="366" spans="1:8">
+    <row r="366" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>10</v>
       </c>
@@ -12287,7 +12307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="367" spans="1:8">
+    <row r="367" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>10</v>
       </c>
@@ -12310,7 +12330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="368" spans="1:8">
+    <row r="368" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>10</v>
       </c>
@@ -12336,7 +12356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="369" spans="1:8">
+    <row r="369" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
         <v>10</v>
       </c>
@@ -12362,7 +12382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="370" spans="1:8">
+    <row r="370" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
         <v>10</v>
       </c>
@@ -12388,7 +12408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="371" spans="1:8">
+    <row r="371" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
         <v>10</v>
       </c>
@@ -12414,7 +12434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="372" spans="1:8">
+    <row r="372" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
         <v>10</v>
       </c>
@@ -12440,7 +12460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="373" spans="1:8">
+    <row r="373" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
         <v>10</v>
       </c>
@@ -12466,7 +12486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="374" spans="1:8">
+    <row r="374" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
         <v>10</v>
       </c>
@@ -12492,7 +12512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="375" spans="1:8">
+    <row r="375" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
         <v>10</v>
       </c>
@@ -12518,7 +12538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="376" spans="1:8">
+    <row r="376" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
         <v>10</v>
       </c>
@@ -12544,7 +12564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="377" spans="1:8">
+    <row r="377" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
         <v>10</v>
       </c>
@@ -12570,7 +12590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="378" spans="1:8">
+    <row r="378" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
         <v>10</v>
       </c>
@@ -12596,7 +12616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="379" spans="1:8">
+    <row r="379" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
         <v>10</v>
       </c>
@@ -12622,7 +12642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="380" spans="1:8">
+    <row r="380" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
         <v>10</v>
       </c>
@@ -12648,7 +12668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="381" spans="1:8">
+    <row r="381" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
         <v>10</v>
       </c>
@@ -12674,7 +12694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="382" spans="1:8">
+    <row r="382" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
         <v>10</v>
       </c>
@@ -12700,7 +12720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="383" spans="1:8">
+    <row r="383" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
         <v>10</v>
       </c>
@@ -12726,7 +12746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="384" spans="1:8">
+    <row r="384" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
         <v>10</v>
       </c>
@@ -12749,7 +12769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="385" spans="1:8">
+    <row r="385" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
         <v>10</v>
       </c>
@@ -12775,7 +12795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="386" spans="1:8">
+    <row r="386" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
         <v>10</v>
       </c>
@@ -12801,7 +12821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="387" spans="1:8">
+    <row r="387" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
         <v>10</v>
       </c>
@@ -12827,7 +12847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="388" spans="1:8">
+    <row r="388" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
         <v>10</v>
       </c>
@@ -12853,7 +12873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="389" spans="1:8">
+    <row r="389" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
         <v>10</v>
       </c>
@@ -12879,7 +12899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="390" spans="1:8">
+    <row r="390" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
         <v>10</v>
       </c>
@@ -12905,7 +12925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="391" spans="1:8">
+    <row r="391" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
         <v>10</v>
       </c>
@@ -12931,7 +12951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="392" spans="1:8">
+    <row r="392" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
         <v>10</v>
       </c>

</xml_diff>